<commit_message>
UPDATE changement de la taille et du format des images pour optimiser le chargement
</commit_message>
<xml_diff>
--- a/assets/panthere-audit-SEO.xlsx
+++ b/assets/panthere-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brahim\Desktop\Openclassrooms\projet_4\la_panthere_site\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80FE801-B21E-415A-9409-8BC33A1D98AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3E27A6-4371-4F0A-A130-9C77CF2B7D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Catégorie</t>
   </si>
@@ -243,7 +243,10 @@
     <t>Le menu sort de l'écran sur la page de contact</t>
   </si>
   <si>
-    <t>Les photos dans la gallerie sont de trop grande qualité</t>
+    <t>https://www.adobe.com/fr/creativecloud/file-types/image/comparison/bmp-vs-jpeg.html#:~:text=Les%20fichiers%20BMP%2C%20qui%20contiennent,et%20de%20moins%20bonne%20qualit%C3%A9.</t>
+  </si>
+  <si>
+    <t>La résolution des images de la gallerie est trop grande. Le format BPM utilisé pour les images 3 et 4 est trop lourd.</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -350,6 +353,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,11 +896,14 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1896,8 +1905,9 @@
     <hyperlink ref="F11" r:id="rId10" location="images-of-text" xr:uid="{52CCABC8-C91F-4CFB-8E0B-419150FE2E45}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{942D296B-BB62-4DA1-B156-4CCFFF5DF9D9}"/>
     <hyperlink ref="F13" r:id="rId12" location="labels-or-instructions" xr:uid="{EB0411C9-25D0-482E-92E0-9276B30B9229}"/>
+    <hyperlink ref="F16" r:id="rId13" location=":~:text=Les%20fichiers%20BMP%2C%20qui%20contiennent,et%20de%20moins%20bonne%20qualit%C3%A9." xr:uid="{884C41CC-9DCC-45A9-B1A6-A2644D154FC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId13"/>
+  <pageSetup orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE ajout de focus visibles aux éléments interactifs
</commit_message>
<xml_diff>
--- a/assets/panthere-audit-SEO.xlsx
+++ b/assets/panthere-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brahim\Desktop\Openclassrooms\projet_4\la_panthere_site\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3E27A6-4371-4F0A-A130-9C77CF2B7D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C134ADF-AF01-4888-A916-DB7138396748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>Catégorie</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>La valeur "Défaut" dans la balise lang n'existe pas</t>
-  </si>
-  <si>
-    <t>Il est nécessaire de préciser clairement la langue du site dans la balise lang car c'est cette information qui déterminera dans quelle langue les lecteurs d'écran vont lire le site.</t>
-  </si>
-  <si>
     <t>Mettre la langue correspondant au site dans la balise lang. En l'occurrence mettre "fr-fr"</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>Les lecteurs d'écran ne bénéficient pas d'un contexte suffisant pour informer aux utilisateurs quelle est la destination ou le rôle du lien</t>
   </si>
   <si>
-    <t>Supprimer le lien vide, ajouter du texte ou bien ajouter une balise aria pour préciser le rôle du lien</t>
-  </si>
-  <si>
-    <t>Préciser la destination du lien avec une balise title</t>
-  </si>
-  <si>
     <t>https://www.w3.org/TR/WCAG21/#link-purpose-in-context</t>
   </si>
   <si>
@@ -87,12 +75,6 @@
     <t>Les headers permettent d'avoir une structure claire et facilitent la navigation au clavier pour les personnes qui utilisent des technologies d'assistance</t>
   </si>
   <si>
-    <t>Structurer le document afin de s'assurer qu'aucun niveau de titre n'est sauté</t>
-  </si>
-  <si>
-    <t>Remplacer les h3 par des h2</t>
-  </si>
-  <si>
     <t>https://www.w3.org/TR/WCAG21/#info-and-relationships</t>
   </si>
   <si>
@@ -105,24 +87,12 @@
     <t>https://dequeuniversity.com/rules/axe/4.4/landmark-one-main?application=AxeChrome</t>
   </si>
   <si>
-    <t>Utiliser des balises sémantiques &lt;html&gt; ainsi que des roles aria pour encapsuler la totalité du code HTML dans une structure claire</t>
-  </si>
-  <si>
-    <t>Mettre le contenu principal de la page dans une balise &lt;main&gt;</t>
-  </si>
-  <si>
     <t>Un fort contraste est nécessaire pour pouvoir lire le texte, surtout pour les personnes qui ont une vue affaiblie</t>
   </si>
   <si>
     <t>Mettre un contraste entre le texte et l'arrière-plan d'au moins 4,5:1 ou 3:1 si le texte est plus gros que 18 point ou si c'est un texte gras de 14 points ou plus</t>
   </si>
   <si>
-    <t>Problèmes de contraste entre les textes et boutons et l'arrière-plan</t>
-  </si>
-  <si>
-    <t>Changer la couleur des textes et des boutons pour que le contraste soit suffisant</t>
-  </si>
-  <si>
     <t>https://www.w3.org/TR/WCAG21/#contrast-minimum</t>
   </si>
   <si>
@@ -135,15 +105,6 @@
     <t>Décrire correctement chaque image individuellement en utilisant l'attribut alt</t>
   </si>
   <si>
-    <t>Changer les alts de chaque image pour qu'il corresponde à l'image en question</t>
-  </si>
-  <si>
-    <t>Plusieurs images ont le même alt. Les alts ne décrivent pas correctement les images</t>
-  </si>
-  <si>
-    <t>La page n'a pas de titre ou de description</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -156,9 +117,6 @@
     <t>Ecrire un titre de la bonne longueur, qui donne envie à l'utilisateur de cliquer. Donner à chaque page un titre et une description uniques. Mettre les mots clés au début du titre et de la description. Decrire correctement aux utilisateurs ce qu'ils vont trouver sur la page.</t>
   </si>
   <si>
-    <t>Ajouter un titre et une description optimisés pour le SEO dans le &lt;head&gt;</t>
-  </si>
-  <si>
     <t>https://moz.com/learn/seo/title-tag#:~:text=A%20title%20tag%20is%20an,%2C%20SEO%2C%20and%20social%20sharing.</t>
   </si>
   <si>
@@ -171,21 +129,12 @@
     <t>Cette pratique est considérée par les moteurs de recherches comme une technique trompeuse et enfreint les règles. Les moteurs de recherche deviennent de plus en plus performants à repérer ce genre de pratiques et peuvent pénaliser les sites qui s'en servent.</t>
   </si>
   <si>
-    <t>Faire en sorte que tous les textes soient visibles par les utilisateurs, à part les textes descriptifs qui servent à l'accessibilité (alt, aria-labels…)</t>
-  </si>
-  <si>
-    <t>Supprimer les textes cachés</t>
-  </si>
-  <si>
     <t>Utilisation répétée des mêmes mots clés dans la balise &lt;meta content="keywords"&gt;</t>
   </si>
   <si>
     <t>L'utilisation excessive des mêmes mots clés n'a pas d'intérêt, mieux vaut privilégier les mots clés différents en lien avec l'activité du site internet.</t>
   </si>
   <si>
-    <t>Trouver plusieurs mots clés différents en lien avec l'activité.</t>
-  </si>
-  <si>
     <t>Supprimer les mots clés qui se répetent et en ajouter d'autres en lien avec l'activité</t>
   </si>
   <si>
@@ -204,9 +153,6 @@
     <t>Si le résultat visuel peut être atteint en utilisant du texte plutôt qu'une image, alors il faut privilégier l'usage de texte afin de permettre aux utilisateurs de l'adapter à leurs besoins.</t>
   </si>
   <si>
-    <t>Remplacer les images de texte par des textes</t>
-  </si>
-  <si>
     <t>https://developers.google.com/search/docs/advanced/guidelines/link-schemes?hl=fr</t>
   </si>
   <si>
@@ -219,9 +165,6 @@
     <t>Renvoyer à des liens d'autres sites uniquement lorsque cela a un sens dans le contexte de la page en question.</t>
   </si>
   <si>
-    <t>Supprimer les liens dans le footer</t>
-  </si>
-  <si>
     <t>Manque des labels aux éléments de formulaire sur la page contact</t>
   </si>
   <si>
@@ -231,22 +174,52 @@
     <t>Pour les utilisateurs de lecteurs d'écran, il est important que les entrées de formulaires contiennent des informations sur leur rôle et sur comment ils doivent être remplis.</t>
   </si>
   <si>
-    <t>Decrire clairement le rôle de l'entrée de formulaire et ce que l'utilisateur doit y insérer</t>
-  </si>
-  <si>
-    <t>Ajouter des labels aux &lt;input&gt; du formulaire de contact</t>
-  </si>
-  <si>
-    <t>Présence d'un bouton "Toggle navigation" inutile sur la page de contact</t>
-  </si>
-  <si>
-    <t>Le menu sort de l'écran sur la page de contact</t>
-  </si>
-  <si>
-    <t>https://www.adobe.com/fr/creativecloud/file-types/image/comparison/bmp-vs-jpeg.html#:~:text=Les%20fichiers%20BMP%2C%20qui%20contiennent,et%20de%20moins%20bonne%20qualit%C3%A9.</t>
-  </si>
-  <si>
     <t>La résolution des images de la gallerie est trop grande. Le format BPM utilisé pour les images 3 et 4 est trop lourd.</t>
+  </si>
+  <si>
+    <t>Ajouter une balise aria-label pour préciser le rôle du lien</t>
+  </si>
+  <si>
+    <t>Structurer le document afin de s'assurer qu'aucun niveau de titre ne soit sauté</t>
+  </si>
+  <si>
+    <t>La valeur "default" pour la balise html lang n'existe pas</t>
+  </si>
+  <si>
+    <t>Il est nécessaire de préciser clairement la langue du site dans la balise html lang car c'est cette information qui déterminera dans quelle langue les lecteurs d'écran vont lire le site.</t>
+  </si>
+  <si>
+    <t>Utiliser des balises sémantiques html (&lt;main&gt;, &lt;header&gt;…) ou bien des roles aria pour encapsuler la totalité du code HTML dans une structure claire</t>
+  </si>
+  <si>
+    <t>Problèmes de contraste insuffisant entre les textes et autres composants et les arrière-plans</t>
+  </si>
+  <si>
+    <t>Plusieurs images ont le même alt et les alts ne décrivent pas correctement les images</t>
+  </si>
+  <si>
+    <t>La page n'a pas de titre ou de meta description</t>
+  </si>
+  <si>
+    <t>Faire en sorte que tous les textes soient visibles par les utilisateurs, à part les textes descriptifs qui servent à l'accessibilité (alt, aria-labels…). Supprimer les listes de mots-clés intempestifs qui n'ajoutent pas de valeur au contenu</t>
+  </si>
+  <si>
+    <t>Lier les labels aux &lt;input&gt; du formulaire de contact</t>
+  </si>
+  <si>
+    <t>https://blog.adobe.com/en/publish/2022/02/02/how-to-optimize-images-for-your-website</t>
+  </si>
+  <si>
+    <t>Pour optimiser les performances d'un site et réduire les temps de chargement, il est important de choisir la bonne taille et le bon format de compression d'une image. Il est inutile d'avoir une image de trop grande qualité si elle est affichée uniquement en miniature sur le site. La réduction de la taille d'une image sert autant à l'optimisation des performances du site qu'à son meilleur classement dans les résultats de recherche par les moteurs comme Google ou Bing.</t>
+  </si>
+  <si>
+    <t>Optimiser la taille et le format des images selon leur utilisation</t>
+  </si>
+  <si>
+    <t>Il n'y a pas d'indicateur de focus sur tous les éléments interactifs du site</t>
+  </si>
+  <si>
+    <t>https://www.deque.com/blog/give-site-focus-tips-designing-usable-focus-indicators/</t>
   </si>
 </sst>
 </file>
@@ -576,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,19 +610,17 @@
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="60" x14ac:dyDescent="0.25">
@@ -657,19 +628,17 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="60" x14ac:dyDescent="0.25">
@@ -677,19 +646,17 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="75" x14ac:dyDescent="0.25">
@@ -697,19 +664,17 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="75" x14ac:dyDescent="0.25">
@@ -717,139 +682,125 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="7" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>51</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="7" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>57</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="7" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="7" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="75" x14ac:dyDescent="0.25">
@@ -857,54 +808,44 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:26" ht="180" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>70</v>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1905,9 +1846,10 @@
     <hyperlink ref="F11" r:id="rId10" location="images-of-text" xr:uid="{52CCABC8-C91F-4CFB-8E0B-419150FE2E45}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{942D296B-BB62-4DA1-B156-4CCFFF5DF9D9}"/>
     <hyperlink ref="F13" r:id="rId12" location="labels-or-instructions" xr:uid="{EB0411C9-25D0-482E-92E0-9276B30B9229}"/>
-    <hyperlink ref="F16" r:id="rId13" location=":~:text=Les%20fichiers%20BMP%2C%20qui%20contiennent,et%20de%20moins%20bonne%20qualit%C3%A9." xr:uid="{884C41CC-9DCC-45A9-B1A6-A2644D154FC7}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{884C41CC-9DCC-45A9-B1A6-A2644D154FC7}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{63D91318-0445-409D-B008-098EAE4452F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId14"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE ajout de balises html sémantiques
</commit_message>
<xml_diff>
--- a/assets/panthere-audit-SEO.xlsx
+++ b/assets/panthere-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brahim\Desktop\Openclassrooms\projet_4\la_panthere_site\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C134ADF-AF01-4888-A916-DB7138396748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C6281E-C7E3-4836-B99D-71F3CB4EE4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Catégorie</t>
   </si>
@@ -147,9 +147,6 @@
     <t>https://www.w3.org/TR/WCAG21/#images-of-text</t>
   </si>
   <si>
-    <t>Le texte doit pouvoir être modifé pour être compris par l'utilisateur. Par exemple, l'utilisateur doit pouvoir changer de police, ce qui n'est pas possible avec une image. De plus, les lecteurs d'écran peuvent lire du texte mais ne peuvent pas lire une image. En termes de SEO, le moteur de recherche utilise les textes pour comprendre le contexte de la page. Si le texte est une image, alors cela rend difficile l'optimisation SEO par mots clés.</t>
-  </si>
-  <si>
     <t>Si le résultat visuel peut être atteint en utilisant du texte plutôt qu'une image, alors il faut privilégier l'usage de texte afin de permettre aux utilisateurs de l'adapter à leurs besoins.</t>
   </si>
   <si>
@@ -220,6 +217,36 @@
   </si>
   <si>
     <t>https://www.deque.com/blog/give-site-focus-tips-designing-usable-focus-indicators/</t>
+  </si>
+  <si>
+    <t>Les personnes qui utilisent des technologies d'assistance bénéficient grandement de la possibilité de se déplacer au sein d'une page sans utiliser la souris. Il est donc important d'indiquer aux utilisateurs quels élements sont actuellement en focus.</t>
+  </si>
+  <si>
+    <t>Ajouter un indicateur de focus aux éléments interactifs</t>
+  </si>
+  <si>
+    <t>Ajouter des balises sémantiques</t>
+  </si>
+  <si>
+    <t>Ajouter des attributs title aux liens</t>
+  </si>
+  <si>
+    <t>SEO &amp; performance</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Bonne pratique : charger les scripts à travers des CDN</t>
+  </si>
+  <si>
+    <t>Les scripts JS sont chargés à partir du serveur lui-même. Certains scripts sont inutiles.</t>
+  </si>
+  <si>
+    <t>Ajouter un fichier .htaccess pour le cache navigateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -549,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,10 +637,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>7</v>
@@ -634,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="7" t="s">
@@ -652,7 +679,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7" t="s">
@@ -670,7 +697,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="7" t="s">
@@ -682,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>18</v>
@@ -700,7 +727,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>22</v>
@@ -718,7 +745,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>26</v>
@@ -742,7 +769,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="s">
@@ -767,7 +794,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -775,10 +802,10 @@
         <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="7" t="s">
@@ -790,17 +817,17 @@
         <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="75" x14ac:dyDescent="0.25">
@@ -808,62 +835,87 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>62</v>
-      </c>
     </row>
-    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="33" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" s="2" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>